<commit_message>
lista 4 - ex 1
</commit_message>
<xml_diff>
--- a/ep01/result_algo.xlsx
+++ b/ep01/result_algo.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\master-data-structures-algorithms\ep01\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{719E0309-9B7E-4B06-8318-92B71A06F823}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F23ED398-E4A5-40A6-86E3-A4BF28F9C1B0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{1FF3D03A-8F0C-48E5-AA25-061DB21A9BE7}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{1FF3D03A-8F0C-48E5-AA25-061DB21A9BE7}"/>
   </bookViews>
   <sheets>
     <sheet name="t(n)" sheetId="16" r:id="rId1"/>
@@ -19,8 +19,8 @@
   </sheets>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="9" r:id="rId4"/>
-    <pivotCache cacheId="12" r:id="rId5"/>
+    <pivotCache cacheId="0" r:id="rId4"/>
+    <pivotCache cacheId="1" r:id="rId5"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -145,7 +145,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="0.0"/>
+    <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -206,7 +206,7 @@
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -537,7 +537,7 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
-        <c:numFmt formatCode="0.00" sourceLinked="1"/>
+        <c:numFmt formatCode="0" sourceLinked="0"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -1284,6 +1284,7 @@
       <c:valAx>
         <c:axId val="1833144064"/>
         <c:scaling>
+          <c:logBase val="2"/>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
@@ -4285,7 +4286,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{680EA2AC-9ABC-441E-8DF4-175144D3133C}" name="Tabela dinâmica12" cacheId="12" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="7" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="7" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="1">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{680EA2AC-9ABC-441E-8DF4-175144D3133C}" name="Tabela dinâmica12" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="7" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="7" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="1">
   <location ref="A3:B15" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="2">
     <pivotField axis="axisRow" showAll="0">
@@ -4378,7 +4379,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{640EF163-5532-4ACF-A0ED-4775897CCAF9}" name="Tabela dinâmica15" cacheId="9" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="7" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="7" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="1">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{640EF163-5532-4ACF-A0ED-4775897CCAF9}" name="Tabela dinâmica15" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="7" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="7" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="1">
   <location ref="A3:B14" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="2">
     <pivotField axis="axisRow" showAll="0">
@@ -4764,8 +4765,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{71C2642E-822E-41D3-A59F-09EFA0ECC521}">
   <dimension ref="A2:C15"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="M18" sqref="M18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4941,7 +4942,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2BD668A8-AA09-409C-B04C-9CF90FA9BCEB}">
   <dimension ref="A2:F14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>

</xml_diff>